<commit_message>
Add Task board, GoodBadTry and modified Sprint Backlog in Lab6
</commit_message>
<xml_diff>
--- a/Lab_6/SprintBacklog.xlsx
+++ b/Lab_6/SprintBacklog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -91,9 +91,6 @@
     <t>ทดสอบ Login ทั้ง 2 วิธี</t>
   </si>
   <si>
-    <t>ศุภกฤต</t>
-  </si>
-  <si>
     <t>ทดสอบแสดงข้อมูลถูกคน</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>ออกแบบหน้าเลือกคณะ/สาขา/ชั้นปี/ภาคการศึกษา</t>
+  </si>
+  <si>
+    <t>ศุภกฤต</t>
   </si>
   <si>
     <t>ทำระบบเลือกวิชา</t>
@@ -1028,9 +1028,7 @@
       <c r="C14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="D14" s="18"/>
       <c r="E14" s="19">
         <v>2.0</v>
       </c>
@@ -1062,9 +1060,7 @@
       <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>24</v>
-      </c>
+      <c r="D15" s="18"/>
       <c r="E15" s="19">
         <v>3.0</v>
       </c>
@@ -1094,11 +1090,9 @@
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="D16" s="18"/>
       <c r="E16" s="23">
         <v>3.0</v>
       </c>
@@ -1129,10 +1123,10 @@
         <v>2.0</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>16</v>
@@ -1166,10 +1160,10 @@
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E18" s="18">
         <v>4.0</v>
@@ -1407,7 +1401,7 @@
         <v>35</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E25" s="18">
         <v>4.0</v>
@@ -1474,9 +1468,7 @@
       <c r="C27" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="24" t="s">
-        <v>31</v>
-      </c>
+      <c r="D27" s="24"/>
       <c r="E27" s="18">
         <v>3.0</v>
       </c>
@@ -28748,17 +28740,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A6:A16"/>
     <mergeCell ref="B6:B16"/>
+    <mergeCell ref="A17:A27"/>
     <mergeCell ref="B17:B27"/>
-    <mergeCell ref="A17:A27"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A6:A16"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:S4"/>
-    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>